<commit_message>
Updated template with empty value
</commit_message>
<xml_diff>
--- a/tfvc_discovery_input_form.xlsx
+++ b/tfvc_discovery_input_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsure\OneDrive\Documents\1_Official\DMAP\New_Development\DevOpsServer2020TOADO_Migration\multiple_project_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A8F99-A712-42D5-BC2F-2C4135A3073B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93929E0-F7FB-4CA5-B85B-F395DA6D3C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Server URL</t>
   </si>
@@ -47,16 +47,7 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>devserver</t>
-  </si>
-  <si>
     <t>http://172.191.4.85/TestCollection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> k3m53c4elwqmaui2xetdmnyfpesxg2qw77k5iakxekvwotpwr2cq</t>
-  </si>
-  <si>
-    <t>qaserver</t>
   </si>
 </sst>
 </file>
@@ -337,7 +328,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -360,30 +351,19 @@
     </row>
     <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{643D8D03-F719-4D55-9590-924B212FB597}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{66377B3B-69A4-4A5D-BA00-EF471B54E97B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added tfvc new excel
</commit_message>
<xml_diff>
--- a/tfvc_discovery_input_form.xlsx
+++ b/tfvc_discovery_input_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsure\OneDrive\Documents\1_Official\DMAP\New_Development\DevOpsServer2020TOADO_Migration\multiple_project_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UPS_Migration\DevOpsServer2020TOADO_Migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46660245-A51A-48FD-9C93-1D8AD05AA2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B390D9-94BF-43AF-9546-7DAFCF174EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Server URL</t>
   </si>
@@ -47,16 +47,10 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>http://128.0.0.1/TestCollection</t>
-  </si>
-  <si>
-    <t>project1</t>
-  </si>
-  <si>
-    <t>adad87adad8ds4449m434344mmnbnbb43434</t>
-  </si>
-  <si>
-    <t>project2</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -334,9 +328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -345,7 +341,7 @@
     <col min="3" max="3" width="46.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -355,34 +351,19 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7756B5D1-095E-49F9-9086-08F351186310}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{DBFB6AA7-4A83-485D-B3A3-2552BC91591C}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>